<commit_message>
Move units to attributes and add volume units
</commit_message>
<xml_diff>
--- a/templates/export/stops.xlsx
+++ b/templates/export/stops.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="992"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -77,6 +77,9 @@
     <t>Report type:</t>
   </si>
   <si>
+    <t>Stops</t>
+  </si>
+  <si>
     <t>Device:</t>
   </si>
   <si>
@@ -92,6 +95,9 @@
     <t>Period:</t>
   </si>
   <si>
+    <t>${dateTool.format("YYYY-MM-dd HH:mm:ss", from, locale, timezone)+" - "+dateTool.format("YYYY-MM-dd HH:mm:ss", to, locale, timezone)}</t>
+  </si>
+  <si>
     <t>Start</t>
   </si>
   <si>
@@ -104,15 +110,12 @@
     <t>Duration</t>
   </si>
   <si>
+    <t>Engine Hours</t>
+  </si>
+  <si>
     <t>Spent Fuel</t>
   </si>
   <si>
-    <t>${dateTool.format("YYYY-MM-dd HH:mm:ss", from, locale, timezone)+" - "+dateTool.format("YYYY-MM-dd HH:mm:ss", to, locale, timezone)}</t>
-  </si>
-  <si>
-    <t>Stops</t>
-  </si>
-  <si>
     <t>${dateTool.format("YYYY-MM-dd HH:mm:ss", stop.startTime, locale, timezone)}</t>
   </si>
   <si>
@@ -122,30 +125,25 @@
     <t>${dateTool.format("YYYY-MM-dd HH:mm:ss",stop.endTime, locale, timezone)}</t>
   </si>
   <si>
-    <t>${stop.spentFuel}</t>
-  </si>
-  <si>
     <t>${stop.duration/86400000.0}</t>
   </si>
   <si>
-    <t>Engine Hours</t>
-  </si>
-  <si>
     <t>${stop.engineHours/86400000.0}</t>
+  </si>
+  <si>
+    <t>${volumeUnit.equals("impGal") ? "".format("%.1f Imp. Gal", stop.spentFuel / 4.546) : volumeUnit.equals("usGal") ? "".format("%.1f U.S. Gal", stop.spentFuel / 3.785) : "".format("%.1f l", stop.spentFuel)}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="5">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
     <numFmt numFmtId="165" formatCode="[h]&quot; h &quot;m&quot; min &quot;s&quot; s&quot;"/>
-    <numFmt numFmtId="166" formatCode="#.##&quot; km&quot;"/>
-    <numFmt numFmtId="167" formatCode="0.##&quot; km/h&quot;"/>
-    <numFmt numFmtId="168" formatCode="[h]&quot; h &quot;m&quot; min&quot;"/>
+    <numFmt numFmtId="166" formatCode="[h]&quot; h &quot;m&quot; min&quot;"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -213,14 +211,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF444444"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
@@ -270,25 +260,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="7"/>
+      <alignment horizontal="left" vertical="center" indent="15"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="15"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+      <alignment horizontal="left" vertical="center" indent="4"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+      <alignment horizontal="left" vertical="center" indent="4"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
@@ -305,25 +295,10 @@
     <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -414,6 +389,159 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>275400</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>151560</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="8314200" cy="9524160"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9360">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>275400</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>151560</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="8314200" cy="9524160"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9360">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>275400</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>151560</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="8314200" cy="9524160"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9360">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -422,8 +550,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
@@ -465,8 +593,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
@@ -508,8 +636,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
@@ -809,7 +937,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -817,13 +945,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875"/>
-    <col min="2" max="2" width="47.28515625"/>
-    <col min="3" max="3" width="20.85546875"/>
-    <col min="4" max="4" width="15.85546875"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125"/>
+    <col min="1" max="1" width="21.140625"/>
+    <col min="2" max="2" width="48.140625"/>
+    <col min="3" max="3" width="21.140625"/>
+    <col min="4" max="4" width="16"/>
+    <col min="5" max="5" width="16.42578125"/>
+    <col min="6" max="6" width="14.7109375"/>
     <col min="7" max="1022" width="8.7109375"/>
+    <col min="1023" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -839,7 +968,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -856,10 +985,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -868,10 +997,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -880,10 +1009,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -900,94 +1029,46 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
     </row>
   </sheetData>
-  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.51181102362204722" footer="0.51181102362204722"/>
+  <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>

</xml_diff>